<commit_message>
Fim run (October 2024)
</commit_message>
<xml_diff>
--- a/projections_check.xlsx
+++ b/projections_check.xlsx
@@ -24755,7 +24755,7 @@
         <v>171.9</v>
       </c>
       <c r="AB203" t="n">
-        <v>884.094</v>
+        <v>321.194</v>
       </c>
       <c r="AC203" t="n">
         <v>0</v>
@@ -24773,10 +24773,10 @@
         <v>0</v>
       </c>
       <c r="AH203" t="n">
-        <v>0</v>
+        <v>160.9</v>
       </c>
       <c r="AI203" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="AJ203" t="n">
         <v>0</v>
@@ -26771,10 +26771,10 @@
         <v>29641.2825253979</v>
       </c>
       <c r="D221" t="n">
-        <v>1104.01593491485</v>
+        <v>1116.01593491485</v>
       </c>
       <c r="E221" t="n">
-        <v>942.52316024042</v>
+        <v>949.52316024042</v>
       </c>
       <c r="F221" t="n">
         <v>0</v>
@@ -26783,7 +26783,7 @@
         <v>0</v>
       </c>
       <c r="H221" t="n">
-        <v>1912.49715834583</v>
+        <v>1885.49715834583</v>
       </c>
       <c r="I221" t="n">
         <v>3170.00819695195</v>
@@ -26801,7 +26801,7 @@
         <v>224.743658420665</v>
       </c>
       <c r="N221" t="n">
-        <v>643.026623793049</v>
+        <v>647.802300992751</v>
       </c>
       <c r="O221" t="n">
         <v>79.275</v>
@@ -26822,16 +26822,16 @@
         <v>0.00495944283065186</v>
       </c>
       <c r="U221" t="n">
-        <v>0.00580887002259489</v>
+        <v>0.00629989728491442</v>
       </c>
       <c r="V221" t="n">
-        <v>0.00534045807802097</v>
+        <v>0.00583217133289549</v>
       </c>
       <c r="W221" t="n">
-        <v>0.00534045807802097</v>
+        <v>0.00583217133289549</v>
       </c>
       <c r="X221" t="n">
-        <v>0.00534045807802097</v>
+        <v>0.00583217133289549</v>
       </c>
       <c r="Y221" t="n">
         <v>0.00524986184574083</v>
@@ -26840,7 +26840,7 @@
         <v>0</v>
       </c>
       <c r="AA221" t="n">
-        <v>22.5</v>
+        <v>35.7</v>
       </c>
       <c r="AB221" t="n">
         <v>467.087025883687</v>
@@ -26870,10 +26870,10 @@
         <v>71.2739115472825</v>
       </c>
       <c r="AK221" t="n">
-        <v>1747.0425587079</v>
+        <v>1763.8182359076</v>
       </c>
       <c r="AL221" t="n">
-        <v>299.496536447372</v>
+        <v>301.72085924767</v>
       </c>
     </row>
     <row r="222">
@@ -26887,10 +26887,10 @@
         <v>29945.3294512391</v>
       </c>
       <c r="D222" t="n">
-        <v>1118.00695702249</v>
+        <v>1130.15903115474</v>
       </c>
       <c r="E222" t="n">
-        <v>945.153641440141</v>
+        <v>952.173177690469</v>
       </c>
       <c r="F222" t="n">
         <v>0</v>
@@ -26899,7 +26899,7 @@
         <v>0</v>
       </c>
       <c r="H222" t="n">
-        <v>1935.05907115805</v>
+        <v>1907.74054956272</v>
       </c>
       <c r="I222" t="n">
         <v>3197.69785327426</v>
@@ -26917,7 +26917,7 @@
         <v>228.029047409692</v>
       </c>
       <c r="N222" t="n">
-        <v>644.821242234442</v>
+        <v>649.610247837752</v>
       </c>
       <c r="O222" t="n">
         <v>79.275</v>
@@ -26956,7 +26956,7 @@
         <v>0</v>
       </c>
       <c r="AA222" t="n">
-        <v>22.5</v>
+        <v>35.7</v>
       </c>
       <c r="AB222" t="n">
         <v>450.668796978304</v>
@@ -26986,10 +26986,10 @@
         <v>74.0562477423516</v>
       </c>
       <c r="AK222" t="n">
-        <v>1762.82819925693</v>
+        <v>1779.76927899249</v>
       </c>
       <c r="AL222" t="n">
-        <v>300.3323992057</v>
+        <v>302.562929852717</v>
       </c>
     </row>
     <row r="223">
@@ -27003,10 +27003,10 @@
         <v>30256.7723869391</v>
       </c>
       <c r="D223" t="n">
-        <v>1132.17528517565</v>
+        <v>1144.48136065195</v>
       </c>
       <c r="E223" t="n">
-        <v>949.791464031177</v>
+        <v>956.830591055415</v>
       </c>
       <c r="F223" t="n">
         <v>0</v>
@@ -27015,7 +27015,7 @@
         <v>0</v>
       </c>
       <c r="H223" t="n">
-        <v>1958.51734850333</v>
+        <v>1930.86765073576</v>
       </c>
       <c r="I223" t="n">
         <v>3225.52033291041</v>
@@ -27033,7 +27033,7 @@
         <v>231.362463474923</v>
       </c>
       <c r="N223" t="n">
-        <v>647.985348463623</v>
+        <v>652.787719668689</v>
       </c>
       <c r="O223" t="n">
         <v>75.203</v>
@@ -27072,7 +27072,7 @@
         <v>0</v>
       </c>
       <c r="AA223" t="n">
-        <v>22.5</v>
+        <v>35.7</v>
       </c>
       <c r="AB223" t="n">
         <v>446.412208570169</v>
@@ -27102,10 +27102,10 @@
         <v>88.4868021619358</v>
       </c>
       <c r="AK223" t="n">
-        <v>1780.16063363927</v>
+        <v>1797.26908032064</v>
       </c>
       <c r="AL223" t="n">
-        <v>301.806115567553</v>
+        <v>304.042871386726</v>
       </c>
     </row>
     <row r="224">
@@ -27119,10 +27119,10 @@
         <v>30562.1364104264</v>
       </c>
       <c r="D224" t="n">
-        <v>1146.52316634625</v>
+        <v>1158.98519480168</v>
       </c>
       <c r="E224" t="n">
-        <v>954.442230288371</v>
+        <v>961.501002762271</v>
       </c>
       <c r="F224" t="n">
         <v>0</v>
@@ -27131,7 +27131,7 @@
         <v>0</v>
       </c>
       <c r="H224" t="n">
-        <v>1982.56689347672</v>
+        <v>1954.57767221682</v>
       </c>
       <c r="I224" t="n">
         <v>3252.33491841196</v>
@@ -27149,7 +27149,7 @@
         <v>234.744608694576</v>
       </c>
       <c r="N224" t="n">
-        <v>651.158285374427</v>
+        <v>655.974059483211</v>
       </c>
       <c r="O224" t="n">
         <v>75.203</v>
@@ -27188,7 +27188,7 @@
         <v>0</v>
       </c>
       <c r="AA224" t="n">
-        <v>22.5</v>
+        <v>35.7</v>
       </c>
       <c r="AB224" t="n">
         <v>449.361288</v>
@@ -27218,10 +27218,10 @@
         <v>103.161764741351</v>
       </c>
       <c r="AK224" t="n">
-        <v>1797.68145172068</v>
+        <v>1814.95925428489</v>
       </c>
       <c r="AL224" t="n">
-        <v>303.283944913944</v>
+        <v>305.52694327906</v>
       </c>
     </row>
     <row r="225">
@@ -27235,10 +27235,10 @@
         <v>30851.8978925676</v>
       </c>
       <c r="D225" t="n">
-        <v>1164.56901748464</v>
+        <v>1177.22719366476</v>
       </c>
       <c r="E225" t="n">
-        <v>962.090282376934</v>
+        <v>969.190826173758</v>
       </c>
       <c r="F225" t="n">
         <v>0</v>
@@ -27247,7 +27247,7 @@
         <v>0</v>
       </c>
       <c r="H225" t="n">
-        <v>1996.72371351529</v>
+        <v>1968.53463096965</v>
       </c>
       <c r="I225" t="n">
         <v>3279.12652002303</v>
@@ -27265,7 +27265,7 @@
         <v>238.176195410118</v>
       </c>
       <c r="N225" t="n">
-        <v>656.376089371782</v>
+        <v>661.220361531208</v>
       </c>
       <c r="O225" t="n">
         <v>75.203</v>
@@ -27304,7 +27304,7 @@
         <v>0</v>
       </c>
       <c r="AA225" t="n">
-        <v>22.5</v>
+        <v>35.7</v>
       </c>
       <c r="AB225" t="n">
         <v>448.453726991034</v>
@@ -27334,10 +27334,10 @@
         <v>109.690951603052</v>
       </c>
       <c r="AK225" t="n">
-        <v>1820.94510685642</v>
+        <v>1838.44755519597</v>
       </c>
       <c r="AL225" t="n">
-        <v>305.714193005152</v>
+        <v>307.97046464255</v>
       </c>
     </row>
     <row r="226">
@@ -27351,10 +27351,10 @@
         <v>31121.5989644067</v>
       </c>
       <c r="D226" t="n">
-        <v>1182.89890365421</v>
+        <v>1195.75631485177</v>
       </c>
       <c r="E226" t="n">
-        <v>969.783592937096</v>
+        <v>976.926155244783</v>
       </c>
       <c r="F226" t="n">
         <v>0</v>
@@ -27363,7 +27363,7 @@
         <v>0</v>
       </c>
       <c r="H226" t="n">
-        <v>2009.5092045073</v>
+        <v>1981.13962064417</v>
       </c>
       <c r="I226" t="n">
         <v>3307.03429149024</v>
@@ -27381,7 +27381,7 @@
         <v>241.657946376297</v>
       </c>
       <c r="N226" t="n">
-        <v>661.624770490695</v>
+        <v>666.497709342163</v>
       </c>
       <c r="O226" t="n">
         <v>75.203</v>
@@ -27420,7 +27420,7 @@
         <v>0</v>
       </c>
       <c r="AA226" t="n">
-        <v>22.5</v>
+        <v>35.7</v>
       </c>
       <c r="AB226" t="n">
         <v>451.587350777436</v>
@@ -27450,10 +27450,10 @@
         <v>134.692196391126</v>
       </c>
       <c r="AK226" t="n">
-        <v>1844.52367414491</v>
+        <v>1862.25402419393</v>
       </c>
       <c r="AL226" t="n">
-        <v>308.158822446401</v>
+        <v>310.42844590262</v>
       </c>
     </row>
     <row r="227">
@@ -27467,10 +27467,10 @@
         <v>31395.1500139805</v>
       </c>
       <c r="D227" t="n">
-        <v>1201.51729546145</v>
+        <v>1214.57707756201</v>
       </c>
       <c r="E227" t="n">
-        <v>977.52242979251</v>
+        <v>984.70725926177</v>
       </c>
       <c r="F227" t="n">
         <v>0</v>
@@ -27479,7 +27479,7 @@
         <v>0</v>
       </c>
       <c r="H227" t="n">
-        <v>2024.68898548318</v>
+        <v>1996.10509851138</v>
       </c>
       <c r="I227" t="n">
         <v>3334.55878226375</v>
@@ -27497,7 +27497,7 @@
         <v>245.190594913367</v>
       </c>
       <c r="N227" t="n">
-        <v>666.904511451069</v>
+        <v>671.806286633939</v>
       </c>
       <c r="O227" t="n">
         <v>75.203</v>
@@ -27536,7 +27536,7 @@
         <v>0</v>
       </c>
       <c r="AA227" t="n">
-        <v>22.5</v>
+        <v>35.7</v>
       </c>
       <c r="AB227" t="n">
         <v>451.948851432976</v>
@@ -27566,10 +27566,10 @@
         <v>155.154681378039</v>
       </c>
       <c r="AK227" t="n">
-        <v>1868.42180691252</v>
+        <v>1886.38336419595</v>
       </c>
       <c r="AL227" t="n">
-        <v>310.617918341441</v>
+        <v>312.900972627831</v>
       </c>
     </row>
     <row r="228">
@@ -27583,10 +27583,10 @@
         <v>31679.947051148</v>
       </c>
       <c r="D228" t="n">
-        <v>1220.42873387852</v>
+        <v>1233.69407212535</v>
       </c>
       <c r="E228" t="n">
-        <v>985.307062351715</v>
+        <v>992.534409104685</v>
       </c>
       <c r="F228" t="n">
         <v>0</v>
@@ -27595,7 +27595,7 @@
         <v>0</v>
       </c>
       <c r="H228" t="n">
-        <v>2038.61125330117</v>
+        <v>2009.83081637402</v>
       </c>
       <c r="I228" t="n">
         <v>3362.393673419</v>
@@ -27613,7 +27613,7 @@
         <v>248.77488506154</v>
       </c>
       <c r="N228" t="n">
-        <v>672.215496054077</v>
+        <v>677.146278211576</v>
       </c>
       <c r="O228" t="n">
         <v>75.203</v>
@@ -27652,7 +27652,7 @@
         <v>0</v>
       </c>
       <c r="AA228" t="n">
-        <v>23.5</v>
+        <v>35.7</v>
       </c>
       <c r="AB228" t="n">
         <v>456.1445332</v>
@@ -27682,10 +27682,10 @@
         <v>162.725745305459</v>
       </c>
       <c r="AK228" t="n">
-        <v>1892.64422993259</v>
+        <v>1910.84035033693</v>
       </c>
       <c r="AL228" t="n">
-        <v>313.091566297638</v>
+        <v>315.388130893108</v>
       </c>
     </row>
     <row r="229">

</xml_diff>

<commit_message>
Forecast sheet edits + FIM run
</commit_message>
<xml_diff>
--- a/projections_check.xlsx
+++ b/projections_check.xlsx
@@ -26617,7 +26617,7 @@
         <v>0</v>
       </c>
       <c r="AD219" t="n">
-        <v>4445.1</v>
+        <v>4417.2</v>
       </c>
       <c r="AE219" t="n">
         <v>2439</v>
@@ -26652,37 +26652,37 @@
         <v>257</v>
       </c>
       <c r="C220" t="n">
-        <v>29349.9</v>
+        <v>29354.3</v>
       </c>
       <c r="D220" t="n">
         <v>1090.2</v>
       </c>
       <c r="E220" t="n">
-        <v>939.9</v>
+        <v>919.4</v>
       </c>
       <c r="F220" t="n">
         <v>35.7</v>
       </c>
       <c r="G220" t="n">
-        <v>4441</v>
+        <v>4424.9</v>
       </c>
       <c r="H220" t="n">
-        <v>1893.8</v>
+        <v>1893.4</v>
       </c>
       <c r="I220" t="n">
-        <v>3141.3</v>
+        <v>3139.2</v>
       </c>
       <c r="J220" t="n">
-        <v>505.549857309427</v>
+        <v>483.1</v>
       </c>
       <c r="K220" t="n">
-        <v>2151.899</v>
+        <v>2152.299</v>
       </c>
       <c r="L220" t="n">
-        <v>159.961884337329</v>
+        <v>164.8</v>
       </c>
       <c r="M220" t="n">
-        <v>217.6</v>
+        <v>221.6</v>
       </c>
       <c r="N220" t="n">
         <v>641.237</v>
@@ -26703,19 +26703,19 @@
         <v>-1</v>
       </c>
       <c r="T220" t="n">
-        <v>0.00375583046035288</v>
+        <v>0.0037233826809977</v>
       </c>
       <c r="U220" t="n">
-        <v>0.00440944881889749</v>
+        <v>0.00608116293155669</v>
       </c>
       <c r="V220" t="n">
-        <v>0.00723457563419982</v>
+        <v>0.00575477607265906</v>
       </c>
       <c r="W220" t="n">
-        <v>0.00724299619663626</v>
+        <v>0.00523456712027648</v>
       </c>
       <c r="X220" t="n">
-        <v>0.00719601681061177</v>
+        <v>0.00792756208803924</v>
       </c>
       <c r="Y220" t="n">
         <v>0.0051977939134229</v>
@@ -26733,10 +26733,10 @@
         <v>0</v>
       </c>
       <c r="AD220" t="n">
-        <v>4504.1</v>
+        <v>4465.4</v>
       </c>
       <c r="AE220" t="n">
-        <v>2478.8</v>
+        <v>2483.3</v>
       </c>
       <c r="AF220" t="n">
         <v>1.365</v>
@@ -26757,7 +26757,7 @@
         <v>1731.437</v>
       </c>
       <c r="AL220" t="n">
-        <v>298.663</v>
+        <v>278.163</v>
       </c>
     </row>
     <row r="221">
@@ -26768,13 +26768,13 @@
         <v>259</v>
       </c>
       <c r="C221" t="n">
-        <v>29641.2825253979</v>
+        <v>29645.7262081059</v>
       </c>
       <c r="D221" t="n">
         <v>1116.01593491485</v>
       </c>
       <c r="E221" t="n">
-        <v>949.52316024042</v>
+        <v>927.689732874973</v>
       </c>
       <c r="F221" t="n">
         <v>0</v>
@@ -26783,25 +26783,25 @@
         <v>0</v>
       </c>
       <c r="H221" t="n">
-        <v>1885.49715834583</v>
+        <v>1885.09320921534</v>
       </c>
       <c r="I221" t="n">
-        <v>3170.00819695195</v>
+        <v>3167.88900514805</v>
       </c>
       <c r="J221" t="n">
-        <v>515.702621440952</v>
+        <v>492.801912246684</v>
       </c>
       <c r="K221" t="n">
-        <v>2160.127</v>
+        <v>2160.527</v>
       </c>
       <c r="L221" t="n">
-        <v>161.167613599023</v>
+        <v>163.15466849793</v>
       </c>
       <c r="M221" t="n">
         <v>224.743658420665</v>
       </c>
       <c r="N221" t="n">
-        <v>647.802300992751</v>
+        <v>647.018687447845</v>
       </c>
       <c r="O221" t="n">
         <v>79.275</v>
@@ -26819,7 +26819,7 @@
         <v>0</v>
       </c>
       <c r="T221" t="n">
-        <v>0.00495944283065186</v>
+        <v>0.00545171502706143</v>
       </c>
       <c r="U221" t="n">
         <v>0.00629989728491442</v>
@@ -26849,10 +26849,10 @@
         <v>0</v>
       </c>
       <c r="AD221" t="n">
-        <v>4552.98820304714</v>
+        <v>4505.15020255048</v>
       </c>
       <c r="AE221" t="n">
-        <v>2512.48563586214</v>
+        <v>2522.33520327819</v>
       </c>
       <c r="AF221" t="n">
         <v>-0.901</v>
@@ -26870,10 +26870,10 @@
         <v>71.2739115472825</v>
       </c>
       <c r="AK221" t="n">
-        <v>1763.8182359076</v>
+        <v>1763.0346223627</v>
       </c>
       <c r="AL221" t="n">
-        <v>301.72085924767</v>
+        <v>280.671045427128</v>
       </c>
     </row>
     <row r="222">
@@ -26884,13 +26884,13 @@
         <v>260</v>
       </c>
       <c r="C222" t="n">
-        <v>29945.3294512391</v>
+        <v>29949.8187152429</v>
       </c>
       <c r="D222" t="n">
         <v>1130.15903115474</v>
       </c>
       <c r="E222" t="n">
-        <v>952.173177690469</v>
+        <v>928.991094574193</v>
       </c>
       <c r="F222" t="n">
         <v>0</v>
@@ -26899,25 +26899,25 @@
         <v>0</v>
       </c>
       <c r="H222" t="n">
-        <v>1907.74054956272</v>
+        <v>1907.3318350055</v>
       </c>
       <c r="I222" t="n">
-        <v>3197.69785327426</v>
+        <v>3195.56015057414</v>
       </c>
       <c r="J222" t="n">
-        <v>526.059279645475</v>
+        <v>502.698664280664</v>
       </c>
       <c r="K222" t="n">
-        <v>2201.67869024</v>
+        <v>2202.093889974</v>
       </c>
       <c r="L222" t="n">
-        <v>162.643685744505</v>
+        <v>164.648939314487</v>
       </c>
       <c r="M222" t="n">
         <v>228.029047409692</v>
       </c>
       <c r="N222" t="n">
-        <v>649.610247837752</v>
+        <v>647.926324245673</v>
       </c>
       <c r="O222" t="n">
         <v>79.275</v>
@@ -26965,10 +26965,10 @@
         <v>0</v>
       </c>
       <c r="AD222" t="n">
-        <v>4626.71543072323</v>
+        <v>4578.04931402487</v>
       </c>
       <c r="AE222" t="n">
-        <v>2538.47766418171</v>
+        <v>2548.44772380158</v>
       </c>
       <c r="AF222" t="n">
         <v>-0.901</v>
@@ -26986,10 +26986,10 @@
         <v>74.0562477423516</v>
       </c>
       <c r="AK222" t="n">
-        <v>1779.76927899249</v>
+        <v>1778.08535540041</v>
       </c>
       <c r="AL222" t="n">
-        <v>302.562929852717</v>
+        <v>281.06477032852</v>
       </c>
     </row>
     <row r="223">
@@ -27000,13 +27000,13 @@
         <v>261</v>
       </c>
       <c r="C223" t="n">
-        <v>30256.7723869391</v>
+        <v>30261.308341014</v>
       </c>
       <c r="D223" t="n">
         <v>1144.48136065195</v>
       </c>
       <c r="E223" t="n">
-        <v>956.830591055415</v>
+        <v>932.294281821561</v>
       </c>
       <c r="F223" t="n">
         <v>0</v>
@@ -27015,25 +27015,25 @@
         <v>0</v>
       </c>
       <c r="H223" t="n">
-        <v>1930.86765073576</v>
+        <v>1930.4539814257</v>
       </c>
       <c r="I223" t="n">
-        <v>3225.52033291041</v>
+        <v>3223.36403051996</v>
       </c>
       <c r="J223" t="n">
-        <v>536.623926649562</v>
+        <v>512.794168994753</v>
       </c>
       <c r="K223" t="n">
-        <v>2208.37869024</v>
+        <v>2208.793889974</v>
       </c>
       <c r="L223" t="n">
-        <v>164.114351032311</v>
+        <v>166.13773661157</v>
       </c>
       <c r="M223" t="n">
         <v>231.362463474923</v>
       </c>
       <c r="N223" t="n">
-        <v>652.787719668689</v>
+        <v>650.230137472713</v>
       </c>
       <c r="O223" t="n">
         <v>75.203</v>
@@ -27081,10 +27081,10 @@
         <v>0</v>
       </c>
       <c r="AD223" t="n">
-        <v>4658.68738402263</v>
+        <v>4609.71515475437</v>
       </c>
       <c r="AE223" t="n">
-        <v>2564.39985834083</v>
+        <v>2574.48894008494</v>
       </c>
       <c r="AF223" t="n">
         <v>-0.901</v>
@@ -27102,10 +27102,10 @@
         <v>88.4868021619358</v>
       </c>
       <c r="AK223" t="n">
-        <v>1797.26908032064</v>
+        <v>1794.71149812467</v>
       </c>
       <c r="AL223" t="n">
-        <v>304.042871386726</v>
+        <v>282.064144348848</v>
       </c>
     </row>
     <row r="224">
@@ -27116,13 +27116,13 @@
         <v>262</v>
       </c>
       <c r="C224" t="n">
-        <v>30562.1364104264</v>
+        <v>30566.7181432502</v>
       </c>
       <c r="D224" t="n">
         <v>1158.98519480168</v>
       </c>
       <c r="E224" t="n">
-        <v>961.501002762271</v>
+        <v>935.602102774806</v>
       </c>
       <c r="F224" t="n">
         <v>0</v>
@@ -27131,25 +27131,25 @@
         <v>0</v>
       </c>
       <c r="H224" t="n">
-        <v>1954.57767221682</v>
+        <v>1954.158923269</v>
       </c>
       <c r="I224" t="n">
-        <v>3252.33491841196</v>
+        <v>3250.16069012155</v>
       </c>
       <c r="J224" t="n">
-        <v>547.400739412603</v>
+        <v>523.092417862893</v>
       </c>
       <c r="K224" t="n">
-        <v>2215.07869024</v>
+        <v>2215.493889974</v>
       </c>
       <c r="L224" t="n">
-        <v>165.049737410218</v>
+        <v>167.08465548067</v>
       </c>
       <c r="M224" t="n">
         <v>234.744608694576</v>
       </c>
       <c r="N224" t="n">
-        <v>655.974059483211</v>
+        <v>652.537182485326</v>
       </c>
       <c r="O224" t="n">
         <v>75.203</v>
@@ -27197,10 +27197,10 @@
         <v>0</v>
       </c>
       <c r="AD224" t="n">
-        <v>4690.90825073696</v>
+        <v>4641.62782503496</v>
       </c>
       <c r="AE224" t="n">
-        <v>2589.31708878998</v>
+        <v>2599.52236547798</v>
       </c>
       <c r="AF224" t="n">
         <v>-0.901</v>
@@ -27218,10 +27218,10 @@
         <v>103.161764741351</v>
       </c>
       <c r="AK224" t="n">
-        <v>1814.95925428489</v>
+        <v>1811.522377287</v>
       </c>
       <c r="AL224" t="n">
-        <v>305.52694327906</v>
+        <v>283.064920289481</v>
       </c>
     </row>
     <row r="225">
@@ -27232,13 +27232,13 @@
         <v>263</v>
       </c>
       <c r="C225" t="n">
-        <v>30851.8978925676</v>
+        <v>30856.5230650801</v>
       </c>
       <c r="D225" t="n">
         <v>1177.22719366476</v>
       </c>
       <c r="E225" t="n">
-        <v>969.190826173758</v>
+        <v>941.843153399173</v>
       </c>
       <c r="F225" t="n">
         <v>0</v>
@@ -27247,25 +27247,25 @@
         <v>0</v>
       </c>
       <c r="H225" t="n">
-        <v>1968.53463096965</v>
+        <v>1968.11289188136</v>
       </c>
       <c r="I225" t="n">
-        <v>3279.12652002303</v>
+        <v>3276.93438119768</v>
       </c>
       <c r="J225" t="n">
-        <v>546.018477284129</v>
+        <v>521.771537588453</v>
       </c>
       <c r="K225" t="n">
-        <v>2205.53969024</v>
+        <v>2205.954889974</v>
       </c>
       <c r="L225" t="n">
-        <v>165.130840275354</v>
+        <v>167.166758272789</v>
       </c>
       <c r="M225" t="n">
         <v>238.176195410118</v>
       </c>
       <c r="N225" t="n">
-        <v>661.220361531208</v>
+        <v>656.890013221912</v>
       </c>
       <c r="O225" t="n">
         <v>75.203</v>
@@ -27313,10 +27313,10 @@
         <v>0</v>
       </c>
       <c r="AD225" t="n">
-        <v>4723.38023384059</v>
+        <v>4673.78951251855</v>
       </c>
       <c r="AE225" t="n">
-        <v>2613.92267757626</v>
+        <v>2624.24639104833</v>
       </c>
       <c r="AF225" t="n">
         <v>-2.15</v>
@@ -27334,10 +27334,10 @@
         <v>109.690951603052</v>
       </c>
       <c r="AK225" t="n">
-        <v>1838.44755519597</v>
+        <v>1834.11720688667</v>
       </c>
       <c r="AL225" t="n">
-        <v>307.97046464255</v>
+        <v>284.953140177262</v>
       </c>
     </row>
     <row r="226">
@@ -27348,13 +27348,13 @@
         <v>264</v>
       </c>
       <c r="C226" t="n">
-        <v>31121.5989644067</v>
+        <v>31126.264569245</v>
       </c>
       <c r="D226" t="n">
         <v>1195.75631485177</v>
       </c>
       <c r="E226" t="n">
-        <v>976.926155244783</v>
+        <v>948.11249448117</v>
       </c>
       <c r="F226" t="n">
         <v>0</v>
@@ -27363,25 +27363,25 @@
         <v>0</v>
       </c>
       <c r="H226" t="n">
-        <v>1981.13962064417</v>
+        <v>1980.71518106142</v>
       </c>
       <c r="I226" t="n">
-        <v>3307.03429149024</v>
+        <v>3304.82349595586</v>
       </c>
       <c r="J226" t="n">
-        <v>544.639705557575</v>
+        <v>520.453992718313</v>
       </c>
       <c r="K226" t="n">
-        <v>2249.29677435552</v>
+        <v>2249.7275234174</v>
       </c>
       <c r="L226" t="n">
-        <v>164.406321346802</v>
+        <v>166.433306663197</v>
       </c>
       <c r="M226" t="n">
         <v>241.657946376297</v>
       </c>
       <c r="N226" t="n">
-        <v>666.497709342163</v>
+        <v>661.262575183405</v>
       </c>
       <c r="O226" t="n">
         <v>75.203</v>
@@ -27429,10 +27429,10 @@
         <v>0</v>
       </c>
       <c r="AD226" t="n">
-        <v>4806.46436496607</v>
+        <v>4755.93289067343</v>
       </c>
       <c r="AE226" t="n">
-        <v>2635.95473940002</v>
+        <v>2646.38928336033</v>
       </c>
       <c r="AF226" t="n">
         <v>0</v>
@@ -27450,10 +27450,10 @@
         <v>134.692196391126</v>
       </c>
       <c r="AK226" t="n">
-        <v>1862.25402419393</v>
+        <v>1857.01889003517</v>
       </c>
       <c r="AL226" t="n">
-        <v>310.42844590262</v>
+        <v>286.849919297766</v>
       </c>
     </row>
     <row r="227">
@@ -27464,13 +27464,13 @@
         <v>265</v>
       </c>
       <c r="C227" t="n">
-        <v>31395.1500139805</v>
+        <v>31399.8566283152</v>
       </c>
       <c r="D227" t="n">
         <v>1214.57707756201</v>
       </c>
       <c r="E227" t="n">
-        <v>984.70725926177</v>
+        <v>954.410254260423</v>
       </c>
       <c r="F227" t="n">
         <v>0</v>
@@ -27479,25 +27479,25 @@
         <v>0</v>
       </c>
       <c r="H227" t="n">
-        <v>1996.10509851138</v>
+        <v>1995.67745272291</v>
       </c>
       <c r="I227" t="n">
-        <v>3334.55878226375</v>
+        <v>3332.32958624848</v>
       </c>
       <c r="J227" t="n">
-        <v>543.264415419196</v>
+        <v>519.139774830117</v>
       </c>
       <c r="K227" t="n">
-        <v>2255.26877435552</v>
+        <v>2255.6995234174</v>
       </c>
       <c r="L227" t="n">
-        <v>164.287370477936</v>
+        <v>166.312889234756</v>
       </c>
       <c r="M227" t="n">
         <v>245.190594913367</v>
       </c>
       <c r="N227" t="n">
-        <v>671.806286633939</v>
+        <v>665.654957810736</v>
       </c>
       <c r="O227" t="n">
         <v>75.203</v>
@@ -27545,10 +27545,10 @@
         <v>0</v>
       </c>
       <c r="AD227" t="n">
-        <v>4839.69520590623</v>
+        <v>4788.84607274818</v>
       </c>
       <c r="AE227" t="n">
-        <v>2658.84952528593</v>
+        <v>2669.39124256</v>
       </c>
       <c r="AF227" t="n">
         <v>0</v>
@@ -27566,10 +27566,10 @@
         <v>155.154681378039</v>
       </c>
       <c r="AK227" t="n">
-        <v>1886.38336419595</v>
+        <v>1880.23203537275</v>
       </c>
       <c r="AL227" t="n">
-        <v>312.900972627831</v>
+        <v>288.755296449687</v>
       </c>
     </row>
     <row r="228">
@@ -27580,13 +27580,13 @@
         <v>266</v>
       </c>
       <c r="C228" t="n">
-        <v>31679.947051148</v>
+        <v>31684.696360925</v>
       </c>
       <c r="D228" t="n">
         <v>1233.69407212535</v>
       </c>
       <c r="E228" t="n">
-        <v>992.534409104685</v>
+        <v>960.736561557861</v>
       </c>
       <c r="F228" t="n">
         <v>0</v>
@@ -27595,25 +27595,25 @@
         <v>0</v>
       </c>
       <c r="H228" t="n">
-        <v>2009.83081637402</v>
+        <v>2009.40022998616</v>
       </c>
       <c r="I228" t="n">
-        <v>3362.393673419</v>
+        <v>3360.14586941614</v>
       </c>
       <c r="J228" t="n">
-        <v>541.892598077503</v>
+        <v>517.828875522779</v>
       </c>
       <c r="K228" t="n">
-        <v>2262.96877435552</v>
+        <v>2263.3995234174</v>
       </c>
       <c r="L228" t="n">
-        <v>164.725325949672</v>
+        <v>166.756244312196</v>
       </c>
       <c r="M228" t="n">
         <v>248.77488506154</v>
       </c>
       <c r="N228" t="n">
-        <v>677.146278211576</v>
+        <v>670.06725095027</v>
       </c>
       <c r="O228" t="n">
         <v>75.203</v>
@@ -27661,10 +27661,10 @@
         <v>0</v>
       </c>
       <c r="AD228" t="n">
-        <v>4873.18514639485</v>
+        <v>4822.01619301344</v>
       </c>
       <c r="AE228" t="n">
-        <v>2682.25778530291</v>
+        <v>2692.90294087333</v>
       </c>
       <c r="AF228" t="n">
         <v>0</v>
@@ -27682,10 +27682,10 @@
         <v>162.725745305459</v>
       </c>
       <c r="AK228" t="n">
-        <v>1910.84035033693</v>
+        <v>1903.76132307562</v>
       </c>
       <c r="AL228" t="n">
-        <v>315.388130893108</v>
+        <v>290.669310607591</v>
       </c>
     </row>
     <row r="229">
@@ -27696,7 +27696,7 @@
         <v>267</v>
       </c>
       <c r="C229" t="n">
-        <v>31967.7835444218</v>
+        <v>31972.5760053022</v>
       </c>
       <c r="D229" t="n">
         <v>0</v>
@@ -27812,7 +27812,7 @@
         <v>268</v>
       </c>
       <c r="C230" t="n">
-        <v>32251.4661143502</v>
+        <v>32256.3011035973</v>
       </c>
       <c r="D230" t="n">
         <v>0</v>
@@ -27928,7 +27928,7 @@
         <v>269</v>
       </c>
       <c r="C231" t="n">
-        <v>32532.5144889865</v>
+        <v>32537.3916116939</v>
       </c>
       <c r="D231" t="n">
         <v>0</v>
@@ -28044,7 +28044,7 @@
         <v>270</v>
       </c>
       <c r="C232" t="n">
-        <v>32816.9062653397</v>
+        <v>32821.8260227347</v>
       </c>
       <c r="D232" t="n">
         <v>0</v>
@@ -28160,7 +28160,7 @@
         <v>271</v>
       </c>
       <c r="C233" t="n">
-        <v>33105.0467042242</v>
+        <v>33110.0096582887</v>
       </c>
       <c r="D233" t="n">
         <v>0</v>
@@ -28276,7 +28276,7 @@
         <v>272</v>
       </c>
       <c r="C234" t="n">
-        <v>33397.5436968611</v>
+        <v>33402.5505007094</v>
       </c>
       <c r="D234" t="n">
         <v>0</v>
@@ -28392,7 +28392,7 @@
         <v>273</v>
       </c>
       <c r="C235" t="n">
-        <v>33697.0314385427</v>
+        <v>33702.0831401952</v>
       </c>
       <c r="D235" t="n">
         <v>0</v>
@@ -28508,7 +28508,7 @@
         <v>274</v>
       </c>
       <c r="C236" t="n">
-        <v>34003.0033532512</v>
+        <v>34008.1009247848</v>
       </c>
       <c r="D236" t="n">
         <v>0</v>
@@ -28624,7 +28624,7 @@
         <v>275</v>
       </c>
       <c r="C237" t="n">
-        <v>34315.3581257832</v>
+        <v>34320.5025240862</v>
       </c>
       <c r="D237" t="n">
         <v>0</v>
@@ -28740,7 +28740,7 @@
         <v>276</v>
       </c>
       <c r="C238" t="n">
-        <v>34633.1839193066</v>
+        <v>34638.3759645689</v>
       </c>
       <c r="D238" t="n">
         <v>0</v>
@@ -28856,7 +28856,7 @@
         <v>277</v>
       </c>
       <c r="C239" t="n">
-        <v>34956.582049025</v>
+        <v>34961.8225766253</v>
       </c>
       <c r="D239" t="n">
         <v>0</v>
@@ -28972,7 +28972,7 @@
         <v>278</v>
       </c>
       <c r="C240" t="n">
-        <v>35284.7419933101</v>
+        <v>35290.0317171173</v>
       </c>
       <c r="D240" t="n">
         <v>0</v>
@@ -29088,7 +29088,7 @@
         <v>279</v>
       </c>
       <c r="C241" t="n">
-        <v>35616.7519153299</v>
+        <v>35622.0914125148</v>
       </c>
       <c r="D241" t="n">
         <v>0</v>
@@ -29204,7 +29204,7 @@
         <v>280</v>
       </c>
       <c r="C242" t="n">
-        <v>35951.8012934561</v>
+        <v>35957.1910196797</v>
       </c>
       <c r="D242" t="n">
         <v>0</v>
@@ -29320,7 +29320,7 @@
         <v>281</v>
       </c>
       <c r="C243" t="n">
-        <v>36290.3967037064</v>
+        <v>36295.8371905733</v>
       </c>
       <c r="D243" t="n">
         <v>0</v>
@@ -29436,7 +29436,7 @@
         <v>282</v>
       </c>
       <c r="C244" t="n">
-        <v>36632.6394612843</v>
+        <v>36638.1312555879</v>
       </c>
       <c r="D244" t="n">
         <v>0</v>
@@ -29552,7 +29552,7 @@
         <v>283</v>
       </c>
       <c r="C245" t="n">
-        <v>36978.4282509864</v>
+        <v>36983.9718843311</v>
       </c>
       <c r="D245" t="n">
         <v>0</v>
@@ -29668,7 +29668,7 @@
         <v>284</v>
       </c>
       <c r="C246" t="n">
-        <v>37327.3578119984</v>
+        <v>37332.953755234</v>
       </c>
       <c r="D246" t="n">
         <v>0</v>
@@ -29784,7 +29784,7 @@
         <v>285</v>
       </c>
       <c r="C247" t="n">
-        <v>37679.5294595238</v>
+        <v>37685.1781986889</v>
       </c>
       <c r="D247" t="n">
         <v>0</v>
@@ -29900,7 +29900,7 @@
         <v>286</v>
       </c>
       <c r="C248" t="n">
-        <v>38035.1458239698</v>
+        <v>38040.8478754802</v>
       </c>
       <c r="D248" t="n">
         <v>0</v>
@@ -30016,7 +30016,7 @@
         <v>287</v>
       </c>
       <c r="C249" t="n">
-        <v>38393.1937533009</v>
+        <v>38398.9494816855</v>
       </c>
       <c r="D249" t="n">
         <v>0</v>
@@ -30132,7 +30132,7 @@
         <v>288</v>
       </c>
       <c r="C250" t="n">
-        <v>38753.6732475171</v>
+        <v>38759.4830173047</v>
       </c>
       <c r="D250" t="n">
         <v>0</v>
@@ -30248,7 +30248,7 @@
         <v>289</v>
       </c>
       <c r="C251" t="n">
-        <v>39117.1921978397</v>
+        <v>39123.0564646914</v>
       </c>
       <c r="D251" t="n">
         <v>0</v>
@@ -30364,7 +30364,7 @@
         <v>290</v>
       </c>
       <c r="C252" t="n">
-        <v>39483.9532346758</v>
+        <v>39489.87248463</v>
       </c>
       <c r="D252" t="n">
         <v>0</v>
@@ -30480,7 +30480,7 @@
         <v>291</v>
       </c>
       <c r="C253" t="n">
-        <v>39853.5510972111</v>
+        <v>39859.5257555516</v>
       </c>
       <c r="D253" t="n">
         <v>0</v>
@@ -30596,7 +30596,7 @@
         <v>292</v>
       </c>
       <c r="C254" t="n">
-        <v>40225.8844702422</v>
+        <v>40231.9149470639</v>
       </c>
       <c r="D254" t="n">
         <v>0</v>
@@ -30712,7 +30712,7 @@
         <v>293</v>
       </c>
       <c r="C255" t="n">
-        <v>40601.1559841761</v>
+        <v>40607.2427199514</v>
       </c>
       <c r="D255" t="n">
         <v>0</v>
@@ -30828,7 +30828,7 @@
         <v>294</v>
       </c>
       <c r="C256" t="n">
-        <v>40979.5682694199</v>
+        <v>40985.7117349985</v>
       </c>
       <c r="D256" t="n">
         <v>0</v>
@@ -30944,7 +30944,7 @@
         <v>295</v>
       </c>
       <c r="C257" t="n">
-        <v>41361.2226411772</v>
+        <v>41367.4233225977</v>
       </c>
       <c r="D257" t="n">
         <v>0</v>
@@ -31060,7 +31060,7 @@
         <v>296</v>
       </c>
       <c r="C258" t="n">
-        <v>41746.4230450586</v>
+        <v>41752.6814739255</v>
       </c>
       <c r="D258" t="n">
         <v>0</v>
@@ -31176,7 +31176,7 @@
         <v>297</v>
       </c>
       <c r="C259" t="n">
-        <v>42134.9668506571</v>
+        <v>42141.2835281975</v>
       </c>
       <c r="D259" t="n">
         <v>0</v>
@@ -31292,7 +31292,7 @@
         <v>298</v>
       </c>
       <c r="C260" t="n">
-        <v>42527.0566883796</v>
+        <v>42533.4321461982</v>
       </c>
       <c r="D260" t="n">
         <v>0</v>

</xml_diff>